<commit_message>
Add: pairwise ids; Update: App structure
</commit_message>
<xml_diff>
--- a/public/asset/Book1.xlsx
+++ b/public/asset/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chihy\Dropbox\Ongoing - Dropbox\app-AHP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ongoing - Dropbox\app-AHP\public\asset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{50B25345-DAC5-4E3C-9A0D-0305652412C4}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2B5FF45-83C9-47EC-A16B-BCE900D4691F}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10238" xr2:uid="{37971D20-4150-4350-954F-912B86F59D3D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10240" xr2:uid="{37971D20-4150-4350-954F-912B86F59D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>aa</t>
   </si>
@@ -437,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA7E53A6-C034-4709-831A-BA74DB0D8F78}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -455,7 +455,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -466,7 +466,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -477,12 +477,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
         <v>2</v>
       </c>
@@ -490,42 +490,50 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B8" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B9" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C10" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>